<commit_message>
final report updated sections of text and markdown formatting
</commit_message>
<xml_diff>
--- a/final_outputs/all_topics_errors_reviewed.xlsx
+++ b/final_outputs/all_topics_errors_reviewed.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manat\OneDrive\Documents\Tim\MIDS\266_NLP\Final Project\w266_final_project\final_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0565EF06-4FD7-49F1-ACA6-B50D73484B2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F051C3F8-C7D2-4661-A3D0-C9029B5FEB9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="4800" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="all_topics_errors" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">all_topics_errors!$A$1:$H$400</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">all_topics_errors!$A$1:$I$400</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="433">
   <si>
     <t>obs_num</t>
   </si>
@@ -1276,15 +1276,9 @@
     <t>index</t>
   </si>
   <si>
-    <t>Our model is wrong</t>
-  </si>
-  <si>
     <t>Unclear</t>
   </si>
   <si>
-    <t>True label is wrong</t>
-  </si>
-  <si>
     <t>Sarcasm</t>
   </si>
   <si>
@@ -1325,6 +1319,21 @@
   </si>
   <si>
     <t>unrelated</t>
+  </si>
+  <si>
+    <t>sarcasm</t>
+  </si>
+  <si>
+    <t>blatant</t>
+  </si>
+  <si>
+    <t>missing_context</t>
+  </si>
+  <si>
+    <t>Our model wrong</t>
+  </si>
+  <si>
+    <t>True label wrong</t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1869,47 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5888,7 +5937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J7" sqref="D7:J7"/>
     </sheetView>
   </sheetViews>
@@ -5909,10 +5958,10 @@
   <sheetData>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5920,27 +5969,27 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>420</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
         <v>421</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>422</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>423</v>
-      </c>
       <c r="K4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -6138,7 +6187,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B11" s="3">
         <v>111</v>
@@ -6178,11 +6227,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I126" sqref="I126"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6214,13 +6264,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6243,7 +6293,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -6266,7 +6316,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -6289,7 +6339,7 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6312,10 +6362,10 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>71</v>
       </c>
@@ -6335,7 +6385,7 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6358,7 +6408,7 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6381,7 +6431,7 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -6404,7 +6454,7 @@
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -6427,7 +6477,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -6450,7 +6500,7 @@
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -6473,10 +6523,10 @@
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -6496,7 +6546,7 @@
         <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -6519,7 +6569,7 @@
         <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -6542,7 +6592,7 @@
         <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -6565,7 +6615,7 @@
         <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -6588,7 +6638,7 @@
         <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -6611,10 +6661,10 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -6634,10 +6684,10 @@
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -6657,10 +6707,10 @@
         <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -6680,10 +6730,10 @@
         <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -6703,10 +6753,10 @@
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -6726,10 +6776,10 @@
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -6749,10 +6799,10 @@
         <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -6772,10 +6822,10 @@
         <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -6795,10 +6845,10 @@
         <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -6818,10 +6868,10 @@
         <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -6841,10 +6891,10 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -6864,10 +6914,10 @@
         <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>31</v>
       </c>
@@ -6887,7 +6937,7 @@
         <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -6910,7 +6960,7 @@
         <v>8</v>
       </c>
       <c r="H31" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -6933,10 +6983,10 @@
         <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>39</v>
       </c>
@@ -6956,10 +7006,10 @@
         <v>8</v>
       </c>
       <c r="H33" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>43</v>
       </c>
@@ -6979,10 +7029,10 @@
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>44</v>
       </c>
@@ -7002,10 +7052,10 @@
         <v>8</v>
       </c>
       <c r="H35" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>50</v>
       </c>
@@ -7025,10 +7075,10 @@
         <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>59</v>
       </c>
@@ -7048,10 +7098,10 @@
         <v>8</v>
       </c>
       <c r="H37" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>65</v>
       </c>
@@ -7071,7 +7121,7 @@
         <v>8</v>
       </c>
       <c r="H38" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -7094,10 +7144,10 @@
         <v>8</v>
       </c>
       <c r="H39" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>73</v>
       </c>
@@ -7117,10 +7167,10 @@
         <v>8</v>
       </c>
       <c r="H40" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>85</v>
       </c>
@@ -7140,10 +7190,10 @@
         <v>8</v>
       </c>
       <c r="H41" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>86</v>
       </c>
@@ -7163,10 +7213,10 @@
         <v>8</v>
       </c>
       <c r="H42" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>89</v>
       </c>
@@ -7186,7 +7236,7 @@
         <v>8</v>
       </c>
       <c r="H43" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -7209,10 +7259,10 @@
         <v>8</v>
       </c>
       <c r="H44" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>97</v>
       </c>
@@ -7232,7 +7282,7 @@
         <v>8</v>
       </c>
       <c r="H45" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -7255,7 +7305,7 @@
         <v>7</v>
       </c>
       <c r="H46" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -7278,7 +7328,7 @@
         <v>7</v>
       </c>
       <c r="H47" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -7301,10 +7351,10 @@
         <v>8</v>
       </c>
       <c r="H48" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -7324,10 +7374,10 @@
         <v>8</v>
       </c>
       <c r="H49" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5</v>
       </c>
@@ -7347,10 +7397,10 @@
         <v>8</v>
       </c>
       <c r="H50" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -7370,10 +7420,10 @@
         <v>8</v>
       </c>
       <c r="H51" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>8</v>
       </c>
@@ -7393,10 +7443,10 @@
         <v>8</v>
       </c>
       <c r="H52" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>11</v>
       </c>
@@ -7416,10 +7466,10 @@
         <v>8</v>
       </c>
       <c r="H53" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>13</v>
       </c>
@@ -7439,10 +7489,10 @@
         <v>8</v>
       </c>
       <c r="H54" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>21</v>
       </c>
@@ -7462,10 +7512,10 @@
         <v>8</v>
       </c>
       <c r="H55" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>22</v>
       </c>
@@ -7485,10 +7535,10 @@
         <v>8</v>
       </c>
       <c r="H56" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>24</v>
       </c>
@@ -7508,7 +7558,7 @@
         <v>8</v>
       </c>
       <c r="H57" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -7531,10 +7581,10 @@
         <v>8</v>
       </c>
       <c r="H58" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>27</v>
       </c>
@@ -7554,10 +7604,10 @@
         <v>8</v>
       </c>
       <c r="H59" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>30</v>
       </c>
@@ -7577,7 +7627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>32</v>
       </c>
@@ -7597,7 +7647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>34</v>
       </c>
@@ -7617,7 +7667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>35</v>
       </c>
@@ -7637,7 +7687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>36</v>
       </c>
@@ -7657,7 +7707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>38</v>
       </c>
@@ -7677,7 +7727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>40</v>
       </c>
@@ -7697,7 +7747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>41</v>
       </c>
@@ -7717,7 +7767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>42</v>
       </c>
@@ -7737,7 +7787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>45</v>
       </c>
@@ -7757,7 +7807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>46</v>
       </c>
@@ -7777,7 +7827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>47</v>
       </c>
@@ -7797,7 +7847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>48</v>
       </c>
@@ -7817,7 +7867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>49</v>
       </c>
@@ -7837,7 +7887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>51</v>
       </c>
@@ -7857,7 +7907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>52</v>
       </c>
@@ -7877,7 +7927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>53</v>
       </c>
@@ -7897,7 +7947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>54</v>
       </c>
@@ -7917,7 +7967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>55</v>
       </c>
@@ -7937,7 +7987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>56</v>
       </c>
@@ -7957,7 +8007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>57</v>
       </c>
@@ -7977,7 +8027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>58</v>
       </c>
@@ -7997,7 +8047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>60</v>
       </c>
@@ -8017,7 +8067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>75</v>
       </c>
@@ -8037,7 +8087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>78</v>
       </c>
@@ -8057,7 +8107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>79</v>
       </c>
@@ -8077,7 +8127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>80</v>
       </c>
@@ -8097,7 +8147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>82</v>
       </c>
@@ -8117,7 +8167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>83</v>
       </c>
@@ -8137,7 +8187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -8157,7 +8207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -8177,7 +8227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8197,7 +8247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>92</v>
       </c>
@@ -8217,7 +8267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>93</v>
       </c>
@@ -8237,7 +8287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>94</v>
       </c>
@@ -8257,7 +8307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>95</v>
       </c>
@@ -8277,7 +8327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>96</v>
       </c>
@@ -8297,7 +8347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>98</v>
       </c>
@@ -8317,7 +8367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>99</v>
       </c>
@@ -8337,7 +8387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>102</v>
       </c>
@@ -8377,7 +8427,7 @@
         <v>10</v>
       </c>
       <c r="H100" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -8400,7 +8450,7 @@
         <v>10</v>
       </c>
       <c r="H101" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -8423,7 +8473,7 @@
         <v>10</v>
       </c>
       <c r="H102" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -8446,7 +8496,7 @@
         <v>10</v>
       </c>
       <c r="H103" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -8800,7 +8850,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>105</v>
       </c>
@@ -8827,7 +8877,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>107</v>
       </c>
@@ -8854,7 +8904,7 @@
         <v>Both wrong</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>109</v>
       </c>
@@ -8881,7 +8931,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>110</v>
       </c>
@@ -8907,6 +8957,9 @@
         <f t="shared" si="0"/>
         <v>True label wrong</v>
       </c>
+      <c r="I120" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
@@ -8935,7 +8988,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>114</v>
       </c>
@@ -8961,8 +9014,11 @@
         <f t="shared" si="0"/>
         <v>True label wrong</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I122" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>116</v>
       </c>
@@ -8989,7 +9045,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>117</v>
       </c>
@@ -9016,7 +9072,7 @@
         <v>Both wrong</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>118</v>
       </c>
@@ -9043,7 +9099,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>119</v>
       </c>
@@ -9070,10 +9126,10 @@
         <v>Both wrong</v>
       </c>
       <c r="I126" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>121</v>
       </c>
@@ -9100,7 +9156,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>123</v>
       </c>
@@ -9127,7 +9183,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>124</v>
       </c>
@@ -9154,7 +9210,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>125</v>
       </c>
@@ -9181,7 +9237,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>126</v>
       </c>
@@ -9208,7 +9264,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>127</v>
       </c>
@@ -9234,8 +9290,11 @@
         <f t="shared" si="0"/>
         <v>True label wrong</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>128</v>
       </c>
@@ -9262,7 +9321,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>129</v>
       </c>
@@ -9289,7 +9348,7 @@
         <v>Both wrong</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>138</v>
       </c>
@@ -9316,7 +9375,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>139</v>
       </c>
@@ -9343,7 +9402,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>140</v>
       </c>
@@ -9370,7 +9429,7 @@
         <v>Both wrong</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>146</v>
       </c>
@@ -9397,7 +9456,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>147</v>
       </c>
@@ -9424,7 +9483,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>148</v>
       </c>
@@ -9451,7 +9510,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>149</v>
       </c>
@@ -9478,7 +9537,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>134</v>
       </c>
@@ -9505,7 +9564,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>144</v>
       </c>
@@ -9532,7 +9591,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>145</v>
       </c>
@@ -9559,7 +9618,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>103</v>
       </c>
@@ -9586,7 +9645,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>104</v>
       </c>
@@ -9613,7 +9672,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>106</v>
       </c>
@@ -9640,7 +9699,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>108</v>
       </c>
@@ -9667,7 +9726,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>112</v>
       </c>
@@ -9694,7 +9753,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>113</v>
       </c>
@@ -9721,7 +9780,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>115</v>
       </c>
@@ -9748,7 +9807,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>120</v>
       </c>
@@ -9775,10 +9834,10 @@
         <v>True label wrong</v>
       </c>
       <c r="I152" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>122</v>
       </c>
@@ -9805,7 +9864,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>130</v>
       </c>
@@ -9859,7 +9918,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>171</v>
       </c>
@@ -9879,7 +9938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>194</v>
       </c>
@@ -9899,7 +9958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -9919,7 +9978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>173</v>
       </c>
@@ -9939,7 +9998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>177</v>
       </c>
@@ -9959,7 +10018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>182</v>
       </c>
@@ -9979,7 +10038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>184</v>
       </c>
@@ -9999,7 +10058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>188</v>
       </c>
@@ -10019,7 +10078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>190</v>
       </c>
@@ -10039,7 +10098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>191</v>
       </c>
@@ -10059,7 +10118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>192</v>
       </c>
@@ -10079,7 +10138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>193</v>
       </c>
@@ -10099,7 +10158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>196</v>
       </c>
@@ -10119,7 +10178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>155</v>
       </c>
@@ -10139,7 +10198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>156</v>
       </c>
@@ -10159,7 +10218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>158</v>
       </c>
@@ -10179,7 +10238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>159</v>
       </c>
@@ -10199,7 +10258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>162</v>
       </c>
@@ -10219,7 +10278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>163</v>
       </c>
@@ -10239,7 +10298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>165</v>
       </c>
@@ -10259,7 +10318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>166</v>
       </c>
@@ -10279,7 +10338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>167</v>
       </c>
@@ -10299,7 +10358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>168</v>
       </c>
@@ -10319,7 +10378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>169</v>
       </c>
@@ -10339,7 +10398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>174</v>
       </c>
@@ -10359,7 +10418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>176</v>
       </c>
@@ -10379,7 +10438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>178</v>
       </c>
@@ -10399,7 +10458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>179</v>
       </c>
@@ -10419,7 +10478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>180</v>
       </c>
@@ -10439,7 +10498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>181</v>
       </c>
@@ -10459,7 +10518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>183</v>
       </c>
@@ -10479,7 +10538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -10499,7 +10558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -10519,7 +10578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>195</v>
       </c>
@@ -10539,7 +10598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>197</v>
       </c>
@@ -10559,7 +10618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>198</v>
       </c>
@@ -10579,7 +10638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>199</v>
       </c>
@@ -10599,7 +10658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>189</v>
       </c>
@@ -10619,7 +10678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>160</v>
       </c>
@@ -10639,7 +10698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>161</v>
       </c>
@@ -10659,7 +10718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>164</v>
       </c>
@@ -10679,7 +10738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>170</v>
       </c>
@@ -10699,7 +10758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>172</v>
       </c>
@@ -10719,7 +10778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>175</v>
       </c>
@@ -10739,7 +10798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>185</v>
       </c>
@@ -10759,7 +10818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>326</v>
       </c>
@@ -10779,7 +10838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>329</v>
       </c>
@@ -10799,7 +10858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>334</v>
       </c>
@@ -10819,7 +10878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>335</v>
       </c>
@@ -10839,7 +10898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>337</v>
       </c>
@@ -10859,7 +10918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>340</v>
       </c>
@@ -10879,7 +10938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>344</v>
       </c>
@@ -10899,7 +10958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>355</v>
       </c>
@@ -10919,7 +10978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>356</v>
       </c>
@@ -10939,7 +10998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>358</v>
       </c>
@@ -10959,7 +11018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>362</v>
       </c>
@@ -10979,7 +11038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>363</v>
       </c>
@@ -10999,7 +11058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>364</v>
       </c>
@@ -11019,7 +11078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>365</v>
       </c>
@@ -11039,7 +11098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>366</v>
       </c>
@@ -11059,7 +11118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>368</v>
       </c>
@@ -11079,7 +11138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>370</v>
       </c>
@@ -11099,7 +11158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>374</v>
       </c>
@@ -11119,7 +11178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>375</v>
       </c>
@@ -11139,7 +11198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>378</v>
       </c>
@@ -11159,7 +11218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>380</v>
       </c>
@@ -11179,7 +11238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>381</v>
       </c>
@@ -11199,7 +11258,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>382</v>
       </c>
@@ -11219,7 +11278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>395</v>
       </c>
@@ -11239,7 +11298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>397</v>
       </c>
@@ -11259,7 +11318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>398</v>
       </c>
@@ -11279,7 +11338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>328</v>
       </c>
@@ -11299,7 +11358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>330</v>
       </c>
@@ -11319,7 +11378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>331</v>
       </c>
@@ -11339,7 +11398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>333</v>
       </c>
@@ -11359,7 +11418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>338</v>
       </c>
@@ -11379,7 +11438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>341</v>
       </c>
@@ -11399,7 +11458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>349</v>
       </c>
@@ -11419,7 +11478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>352</v>
       </c>
@@ -11439,7 +11498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>353</v>
       </c>
@@ -11459,7 +11518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>367</v>
       </c>
@@ -11479,7 +11538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>369</v>
       </c>
@@ -11499,7 +11558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>377</v>
       </c>
@@ -11519,7 +11578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>396</v>
       </c>
@@ -11539,7 +11598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>295</v>
       </c>
@@ -11559,7 +11618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>297</v>
       </c>
@@ -11579,7 +11638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>298</v>
       </c>
@@ -11599,7 +11658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>303</v>
       </c>
@@ -11619,7 +11678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>304</v>
       </c>
@@ -11639,7 +11698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>309</v>
       </c>
@@ -11659,7 +11718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>312</v>
       </c>
@@ -11679,7 +11738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>314</v>
       </c>
@@ -11699,7 +11758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>315</v>
       </c>
@@ -11719,7 +11778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>316</v>
       </c>
@@ -11739,7 +11798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>318</v>
       </c>
@@ -11759,7 +11818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>321</v>
       </c>
@@ -11779,7 +11838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>322</v>
       </c>
@@ -11799,7 +11858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>332</v>
       </c>
@@ -11819,7 +11878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>336</v>
       </c>
@@ -11839,7 +11898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>339</v>
       </c>
@@ -11859,7 +11918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>342</v>
       </c>
@@ -11879,7 +11938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>343</v>
       </c>
@@ -11899,7 +11958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>348</v>
       </c>
@@ -11919,7 +11978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>357</v>
       </c>
@@ -11939,7 +11998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>359</v>
       </c>
@@ -11959,7 +12018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>360</v>
       </c>
@@ -11979,7 +12038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>373</v>
       </c>
@@ -11999,7 +12058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>376</v>
       </c>
@@ -12019,7 +12078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>379</v>
       </c>
@@ -12039,7 +12098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>383</v>
       </c>
@@ -12059,7 +12118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>385</v>
       </c>
@@ -12079,7 +12138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>386</v>
       </c>
@@ -12099,7 +12158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>390</v>
       </c>
@@ -12119,7 +12178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>391</v>
       </c>
@@ -12139,7 +12198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>394</v>
       </c>
@@ -12159,7 +12218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>327</v>
       </c>
@@ -12179,7 +12238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>351</v>
       </c>
@@ -12199,7 +12258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>372</v>
       </c>
@@ -12219,7 +12278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>296</v>
       </c>
@@ -12239,7 +12298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>299</v>
       </c>
@@ -12259,7 +12318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>300</v>
       </c>
@@ -12279,7 +12338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>301</v>
       </c>
@@ -12299,7 +12358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>302</v>
       </c>
@@ -12319,7 +12378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>305</v>
       </c>
@@ -12339,7 +12398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>306</v>
       </c>
@@ -12359,7 +12418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>307</v>
       </c>
@@ -12379,7 +12438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>308</v>
       </c>
@@ -12399,7 +12458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>310</v>
       </c>
@@ -12419,7 +12478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>311</v>
       </c>
@@ -12439,7 +12498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>313</v>
       </c>
@@ -12459,7 +12518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>317</v>
       </c>
@@ -12479,7 +12538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>319</v>
       </c>
@@ -12499,7 +12558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>320</v>
       </c>
@@ -12519,7 +12578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>323</v>
       </c>
@@ -12539,7 +12598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>324</v>
       </c>
@@ -12559,7 +12618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>345</v>
       </c>
@@ -12579,7 +12638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>371</v>
       </c>
@@ -12599,7 +12658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>384</v>
       </c>
@@ -12619,7 +12678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>387</v>
       </c>
@@ -12639,7 +12698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>388</v>
       </c>
@@ -12659,7 +12718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>389</v>
       </c>
@@ -12679,7 +12738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>392</v>
       </c>
@@ -12699,7 +12758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>393</v>
       </c>
@@ -12719,7 +12778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>325</v>
       </c>
@@ -12739,7 +12798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>346</v>
       </c>
@@ -12759,7 +12818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>347</v>
       </c>
@@ -12779,7 +12838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>350</v>
       </c>
@@ -12799,7 +12858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>354</v>
       </c>
@@ -12819,7 +12878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>361</v>
       </c>
@@ -12839,7 +12898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>399</v>
       </c>
@@ -12859,7 +12918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>231</v>
       </c>
@@ -12879,7 +12938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>233</v>
       </c>
@@ -12899,7 +12958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>235</v>
       </c>
@@ -12919,7 +12978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>238</v>
       </c>
@@ -12939,7 +12998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>240</v>
       </c>
@@ -12959,7 +13018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>242</v>
       </c>
@@ -12979,7 +13038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>248</v>
       </c>
@@ -12999,7 +13058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>250</v>
       </c>
@@ -13019,7 +13078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>252</v>
       </c>
@@ -13039,7 +13098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>258</v>
       </c>
@@ -13059,7 +13118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>274</v>
       </c>
@@ -13079,7 +13138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>275</v>
       </c>
@@ -13099,7 +13158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>294</v>
       </c>
@@ -13119,7 +13178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>221</v>
       </c>
@@ -13139,7 +13198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>223</v>
       </c>
@@ -13159,7 +13218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>225</v>
       </c>
@@ -13179,7 +13238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>226</v>
       </c>
@@ -13199,7 +13258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>227</v>
       </c>
@@ -13219,7 +13278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>228</v>
       </c>
@@ -13239,7 +13298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>230</v>
       </c>
@@ -13259,7 +13318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>232</v>
       </c>
@@ -13279,7 +13338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>234</v>
       </c>
@@ -13299,7 +13358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>236</v>
       </c>
@@ -13319,7 +13378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>241</v>
       </c>
@@ -13339,7 +13398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>249</v>
       </c>
@@ -13359,7 +13418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>254</v>
       </c>
@@ -13379,7 +13438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>256</v>
       </c>
@@ -13399,7 +13458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>261</v>
       </c>
@@ -13419,7 +13478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>262</v>
       </c>
@@ -13439,7 +13498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>266</v>
       </c>
@@ -13459,7 +13518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>267</v>
       </c>
@@ -13479,7 +13538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>270</v>
       </c>
@@ -13499,7 +13558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>271</v>
       </c>
@@ -13519,7 +13578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>272</v>
       </c>
@@ -13539,7 +13598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>279</v>
       </c>
@@ -13559,7 +13618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>209</v>
       </c>
@@ -13579,7 +13638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>212</v>
       </c>
@@ -13599,7 +13658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>215</v>
       </c>
@@ -13619,7 +13678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>216</v>
       </c>
@@ -13639,7 +13698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>222</v>
       </c>
@@ -13659,7 +13718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>224</v>
       </c>
@@ -13679,7 +13738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>243</v>
       </c>
@@ -13699,7 +13758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>245</v>
       </c>
@@ -13719,7 +13778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>251</v>
       </c>
@@ -13739,7 +13798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>263</v>
       </c>
@@ -13759,7 +13818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>265</v>
       </c>
@@ -13779,7 +13838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>268</v>
       </c>
@@ -13799,7 +13858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>280</v>
       </c>
@@ -13819,7 +13878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>286</v>
       </c>
@@ -13839,7 +13898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>287</v>
       </c>
@@ -13859,7 +13918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>288</v>
       </c>
@@ -13879,7 +13938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>289</v>
       </c>
@@ -13899,7 +13958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>291</v>
       </c>
@@ -13919,7 +13978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>293</v>
       </c>
@@ -13939,7 +13998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>239</v>
       </c>
@@ -13959,7 +14018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>200</v>
       </c>
@@ -13979,7 +14038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>201</v>
       </c>
@@ -13999,7 +14058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>202</v>
       </c>
@@ -14019,7 +14078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>203</v>
       </c>
@@ -14039,7 +14098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>204</v>
       </c>
@@ -14059,7 +14118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>205</v>
       </c>
@@ -14079,7 +14138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>206</v>
       </c>
@@ -14099,7 +14158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>207</v>
       </c>
@@ -14119,7 +14178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>208</v>
       </c>
@@ -14139,7 +14198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>210</v>
       </c>
@@ -14159,7 +14218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>211</v>
       </c>
@@ -14179,7 +14238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>213</v>
       </c>
@@ -14199,7 +14258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>214</v>
       </c>
@@ -14219,7 +14278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>217</v>
       </c>
@@ -14239,7 +14298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>218</v>
       </c>
@@ -14259,7 +14318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>219</v>
       </c>
@@ -14279,7 +14338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>220</v>
       </c>
@@ -14299,7 +14358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>244</v>
       </c>
@@ -14319,7 +14378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>246</v>
       </c>
@@ -14339,7 +14398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>253</v>
       </c>
@@ -14359,7 +14418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>257</v>
       </c>
@@ -14379,7 +14438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>260</v>
       </c>
@@ -14399,7 +14458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>264</v>
       </c>
@@ -14419,7 +14478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>269</v>
       </c>
@@ -14439,7 +14498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>276</v>
       </c>
@@ -14459,7 +14518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>277</v>
       </c>
@@ -14479,7 +14538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>281</v>
       </c>
@@ -14499,7 +14558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>282</v>
       </c>
@@ -14519,7 +14578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>283</v>
       </c>
@@ -14539,7 +14598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>284</v>
       </c>
@@ -14559,7 +14618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>285</v>
       </c>
@@ -14579,7 +14638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>290</v>
       </c>
@@ -14599,7 +14658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>292</v>
       </c>
@@ -14619,7 +14678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>229</v>
       </c>
@@ -14639,7 +14698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>237</v>
       </c>
@@ -14659,7 +14718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>247</v>
       </c>
@@ -14679,7 +14738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>255</v>
       </c>
@@ -14699,7 +14758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>259</v>
       </c>
@@ -14719,7 +14778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>273</v>
       </c>
@@ -14739,7 +14798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>278</v>
       </c>
@@ -14760,133 +14819,139 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H400" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:I400" xr:uid="{F2932DD1-FA9E-416E-B4CD-BA827FBD2940}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Our model wrong"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataConsolidate/>
-  <conditionalFormatting sqref="H2:H4 H13 H29 H31:H33 H35 H37:H47 H100:H101 H57:H59 I152 E2:G400 I126">
-    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="Favor">
+  <conditionalFormatting sqref="H2:H4 H13 H29 H31:H33 H35 H37:H47 H57:H59 I152 E2:G400 I126 I120 I122 I132 H100:H101">
+    <cfRule type="containsText" dxfId="39" priority="47" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="37" priority="43" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="36" priority="44" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Favor">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",H36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Against">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Against">
       <formula>NOT(ISERROR(SEARCH("Against",H36)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish error analysis + formatting tweaks
</commit_message>
<xml_diff>
--- a/final_outputs/all_topics_errors_reviewed.xlsx
+++ b/final_outputs/all_topics_errors_reviewed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manat\OneDrive\Documents\Tim\MIDS\266_NLP\Final Project\w266_final_project\final_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A420A7-36F2-4A01-A3FE-F0D0115E86F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7AFEAB-37B3-4753-89AA-2F3E6D331C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4800" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="433">
   <si>
     <t>obs_num</t>
   </si>
@@ -5901,22 +5901,22 @@
       <selection activeCell="J7" sqref="D7:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>422</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>416</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>111</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>164</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>306</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>210</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>417</v>
       </c>
@@ -6189,21 +6189,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D407" sqref="D407"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="141.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="8" max="8" width="37.5546875" customWidth="1"/>
+    <col min="4" max="4" width="141.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>412</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>61</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>66</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>68</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>70</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>71</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>72</v>
       </c>
@@ -6370,7 +6370,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>76</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>77</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>81</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>84</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>101</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>16</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>17</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>18</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>19</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>63</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -6692,7 +6692,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -6807,7 +6807,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>31</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>33</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>37</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>39</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>43</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>44</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>50</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>59</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>65</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>67</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>73</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>85</v>
       </c>
@@ -7152,7 +7152,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>86</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>89</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>91</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>97</v>
       </c>
@@ -7244,7 +7244,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>14</v>
       </c>
@@ -7267,7 +7267,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>62</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>8</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>11</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>13</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>21</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>22</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>24</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>26</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>27</v>
       </c>
@@ -7566,7 +7566,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>30</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>32</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>34</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>35</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>36</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>38</v>
       </c>
@@ -7686,7 +7686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>40</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>41</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>42</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>45</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>46</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>47</v>
       </c>
@@ -7806,7 +7806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>48</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>49</v>
       </c>
@@ -7846,7 +7846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>51</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>52</v>
       </c>
@@ -7886,7 +7886,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>53</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>54</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>55</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>56</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>57</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>58</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>60</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>75</v>
       </c>
@@ -8046,7 +8046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>78</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>79</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>80</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>82</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>83</v>
       </c>
@@ -8146,7 +8146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>92</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>93</v>
       </c>
@@ -8246,7 +8246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>94</v>
       </c>
@@ -8266,7 +8266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>95</v>
       </c>
@@ -8286,7 +8286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>96</v>
       </c>
@@ -8306,7 +8306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>98</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>99</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>102</v>
       </c>
@@ -8366,7 +8366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>64</v>
       </c>
@@ -8389,7 +8389,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>69</v>
       </c>
@@ -8412,7 +8412,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>74</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>100</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>131</v>
       </c>
@@ -8485,7 +8485,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>133</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>137</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>142</v>
       </c>
@@ -8566,7 +8566,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>143</v>
       </c>
@@ -8593,7 +8593,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>151</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>152</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>154</v>
       </c>
@@ -8674,7 +8674,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>132</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>135</v>
       </c>
@@ -8721,14 +8721,14 @@
         <v>7</v>
       </c>
       <c r="G113" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="0"/>
-        <v>Our model wrong</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+        <v>True label wrong</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>136</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>141</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>150</v>
       </c>
@@ -8809,7 +8809,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>105</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>107</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>Both wrong</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>109</v>
       </c>
@@ -8890,7 +8890,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>110</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>111</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>114</v>
       </c>
@@ -8977,7 +8977,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>116</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>117</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>Both wrong</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>118</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>119</v>
       </c>
@@ -9084,11 +9084,8 @@
         <f t="shared" si="0"/>
         <v>Both wrong</v>
       </c>
-      <c r="I126" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>121</v>
       </c>
@@ -9115,7 +9112,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>123</v>
       </c>
@@ -9142,7 +9139,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>124</v>
       </c>
@@ -9169,7 +9166,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>125</v>
       </c>
@@ -9196,7 +9193,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>126</v>
       </c>
@@ -9223,7 +9220,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>127</v>
       </c>
@@ -9253,7 +9250,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>128</v>
       </c>
@@ -9280,7 +9277,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>129</v>
       </c>
@@ -9307,7 +9304,7 @@
         <v>Both wrong</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>138</v>
       </c>
@@ -9334,7 +9331,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>139</v>
       </c>
@@ -9361,7 +9358,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>140</v>
       </c>
@@ -9388,7 +9385,7 @@
         <v>Both wrong</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>146</v>
       </c>
@@ -9415,7 +9412,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>147</v>
       </c>
@@ -9442,7 +9439,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>148</v>
       </c>
@@ -9462,14 +9459,14 @@
         <v>8</v>
       </c>
       <c r="G140" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H140" t="str">
         <f t="shared" si="0"/>
-        <v>Our model wrong</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+        <v>Both wrong</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>149</v>
       </c>
@@ -9495,8 +9492,11 @@
         <f t="shared" si="0"/>
         <v>Our model wrong</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I141" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>134</v>
       </c>
@@ -9523,7 +9523,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>144</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>145</v>
       </c>
@@ -9577,7 +9577,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>103</v>
       </c>
@@ -9604,7 +9604,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>104</v>
       </c>
@@ -9631,7 +9631,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>106</v>
       </c>
@@ -9658,7 +9658,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>108</v>
       </c>
@@ -9684,8 +9684,11 @@
         <f t="shared" si="0"/>
         <v>True label wrong</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I148" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>112</v>
       </c>
@@ -9712,7 +9715,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>113</v>
       </c>
@@ -9739,7 +9742,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>115</v>
       </c>
@@ -9766,7 +9769,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>120</v>
       </c>
@@ -9796,7 +9799,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>122</v>
       </c>
@@ -9823,7 +9826,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>130</v>
       </c>
@@ -9850,7 +9853,7 @@
         <v>True label wrong</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
@@ -9877,7 +9880,7 @@
         <v>Our model wrong</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>171</v>
       </c>
@@ -9897,7 +9900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>194</v>
       </c>
@@ -9917,7 +9920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -9937,7 +9940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>173</v>
       </c>
@@ -9957,7 +9960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>177</v>
       </c>
@@ -9977,7 +9980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>182</v>
       </c>
@@ -9997,7 +10000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>184</v>
       </c>
@@ -10017,7 +10020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>188</v>
       </c>
@@ -10037,7 +10040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>190</v>
       </c>
@@ -10057,7 +10060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>191</v>
       </c>
@@ -10077,7 +10080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>192</v>
       </c>
@@ -10097,7 +10100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>193</v>
       </c>
@@ -10117,7 +10120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>196</v>
       </c>
@@ -10137,7 +10140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>155</v>
       </c>
@@ -10157,7 +10160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>156</v>
       </c>
@@ -10177,7 +10180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>158</v>
       </c>
@@ -10197,7 +10200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>159</v>
       </c>
@@ -10217,7 +10220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>162</v>
       </c>
@@ -10237,7 +10240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>163</v>
       </c>
@@ -10257,7 +10260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>165</v>
       </c>
@@ -10277,7 +10280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>166</v>
       </c>
@@ -10297,7 +10300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>167</v>
       </c>
@@ -10317,7 +10320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>168</v>
       </c>
@@ -10337,7 +10340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>169</v>
       </c>
@@ -10357,7 +10360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>174</v>
       </c>
@@ -10377,7 +10380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>176</v>
       </c>
@@ -10397,7 +10400,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>178</v>
       </c>
@@ -10417,7 +10420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>179</v>
       </c>
@@ -10437,7 +10440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>180</v>
       </c>
@@ -10457,7 +10460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>181</v>
       </c>
@@ -10477,7 +10480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>183</v>
       </c>
@@ -10497,7 +10500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -10517,7 +10520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -10537,7 +10540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>195</v>
       </c>
@@ -10557,7 +10560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>197</v>
       </c>
@@ -10577,7 +10580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>198</v>
       </c>
@@ -10597,7 +10600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>199</v>
       </c>
@@ -10617,7 +10620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>189</v>
       </c>
@@ -10637,7 +10640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>160</v>
       </c>
@@ -10657,7 +10660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>161</v>
       </c>
@@ -10677,7 +10680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>164</v>
       </c>
@@ -10697,7 +10700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>170</v>
       </c>
@@ -10717,7 +10720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>172</v>
       </c>
@@ -10737,7 +10740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>175</v>
       </c>
@@ -10757,7 +10760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>185</v>
       </c>
@@ -10777,7 +10780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>326</v>
       </c>
@@ -10797,7 +10800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>329</v>
       </c>
@@ -10817,7 +10820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>334</v>
       </c>
@@ -10837,7 +10840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>335</v>
       </c>
@@ -10857,7 +10860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>337</v>
       </c>
@@ -10877,7 +10880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>340</v>
       </c>
@@ -10897,7 +10900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>344</v>
       </c>
@@ -10917,7 +10920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>355</v>
       </c>
@@ -10937,7 +10940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>356</v>
       </c>
@@ -10957,7 +10960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>358</v>
       </c>
@@ -10977,7 +10980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>362</v>
       </c>
@@ -10997,7 +11000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>363</v>
       </c>
@@ -11017,7 +11020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>364</v>
       </c>
@@ -11037,7 +11040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>365</v>
       </c>
@@ -11057,7 +11060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>366</v>
       </c>
@@ -11077,7 +11080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>368</v>
       </c>
@@ -11097,7 +11100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>370</v>
       </c>
@@ -11117,7 +11120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>374</v>
       </c>
@@ -11137,7 +11140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>375</v>
       </c>
@@ -11157,7 +11160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>378</v>
       </c>
@@ -11177,7 +11180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>380</v>
       </c>
@@ -11197,7 +11200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>381</v>
       </c>
@@ -11217,7 +11220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>382</v>
       </c>
@@ -11237,7 +11240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>395</v>
       </c>
@@ -11257,7 +11260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>397</v>
       </c>
@@ -11277,7 +11280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>398</v>
       </c>
@@ -11297,7 +11300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>328</v>
       </c>
@@ -11317,7 +11320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>330</v>
       </c>
@@ -11337,7 +11340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>331</v>
       </c>
@@ -11357,7 +11360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>333</v>
       </c>
@@ -11377,7 +11380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>338</v>
       </c>
@@ -11397,7 +11400,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>341</v>
       </c>
@@ -11417,7 +11420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>349</v>
       </c>
@@ -11437,7 +11440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>352</v>
       </c>
@@ -11457,7 +11460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>353</v>
       </c>
@@ -11477,7 +11480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>367</v>
       </c>
@@ -11497,7 +11500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>369</v>
       </c>
@@ -11517,7 +11520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>377</v>
       </c>
@@ -11537,7 +11540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>396</v>
       </c>
@@ -11557,7 +11560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>295</v>
       </c>
@@ -11577,7 +11580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>297</v>
       </c>
@@ -11597,7 +11600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>298</v>
       </c>
@@ -11617,7 +11620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>303</v>
       </c>
@@ -11637,7 +11640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>304</v>
       </c>
@@ -11657,7 +11660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>309</v>
       </c>
@@ -11677,7 +11680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>312</v>
       </c>
@@ -11697,7 +11700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>314</v>
       </c>
@@ -11717,7 +11720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>315</v>
       </c>
@@ -11737,7 +11740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>316</v>
       </c>
@@ -11757,7 +11760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>318</v>
       </c>
@@ -11777,7 +11780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>321</v>
       </c>
@@ -11797,7 +11800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>322</v>
       </c>
@@ -11817,7 +11820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>332</v>
       </c>
@@ -11837,7 +11840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>336</v>
       </c>
@@ -11857,7 +11860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>339</v>
       </c>
@@ -11877,7 +11880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>342</v>
       </c>
@@ -11897,7 +11900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>343</v>
       </c>
@@ -11917,7 +11920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>348</v>
       </c>
@@ -11937,7 +11940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>357</v>
       </c>
@@ -11957,7 +11960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>359</v>
       </c>
@@ -11977,7 +11980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>360</v>
       </c>
@@ -11997,7 +12000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>373</v>
       </c>
@@ -12017,7 +12020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>376</v>
       </c>
@@ -12037,7 +12040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>379</v>
       </c>
@@ -12057,7 +12060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>383</v>
       </c>
@@ -12077,7 +12080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>385</v>
       </c>
@@ -12097,7 +12100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>386</v>
       </c>
@@ -12117,7 +12120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>390</v>
       </c>
@@ -12137,7 +12140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>391</v>
       </c>
@@ -12157,7 +12160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>394</v>
       </c>
@@ -12177,7 +12180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>327</v>
       </c>
@@ -12197,7 +12200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>351</v>
       </c>
@@ -12217,7 +12220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>372</v>
       </c>
@@ -12237,7 +12240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>296</v>
       </c>
@@ -12257,7 +12260,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>299</v>
       </c>
@@ -12277,7 +12280,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>300</v>
       </c>
@@ -12297,7 +12300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>301</v>
       </c>
@@ -12317,7 +12320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>302</v>
       </c>
@@ -12337,7 +12340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>305</v>
       </c>
@@ -12357,7 +12360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>306</v>
       </c>
@@ -12377,7 +12380,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>307</v>
       </c>
@@ -12397,7 +12400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>308</v>
       </c>
@@ -12417,7 +12420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>310</v>
       </c>
@@ -12437,7 +12440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>311</v>
       </c>
@@ -12457,7 +12460,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>313</v>
       </c>
@@ -12477,7 +12480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>317</v>
       </c>
@@ -12497,7 +12500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>319</v>
       </c>
@@ -12517,7 +12520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>320</v>
       </c>
@@ -12537,7 +12540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>323</v>
       </c>
@@ -12557,7 +12560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>324</v>
       </c>
@@ -12577,7 +12580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>345</v>
       </c>
@@ -12597,7 +12600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>371</v>
       </c>
@@ -12617,7 +12620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>384</v>
       </c>
@@ -12637,7 +12640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>387</v>
       </c>
@@ -12657,7 +12660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>388</v>
       </c>
@@ -12677,7 +12680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>389</v>
       </c>
@@ -12697,7 +12700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>392</v>
       </c>
@@ -12717,7 +12720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>393</v>
       </c>
@@ -12737,7 +12740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>325</v>
       </c>
@@ -12757,7 +12760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>346</v>
       </c>
@@ -12777,7 +12780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>347</v>
       </c>
@@ -12797,7 +12800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>350</v>
       </c>
@@ -12817,7 +12820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>354</v>
       </c>
@@ -12837,7 +12840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>361</v>
       </c>
@@ -12857,7 +12860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>399</v>
       </c>
@@ -12877,7 +12880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>231</v>
       </c>
@@ -12897,7 +12900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>233</v>
       </c>
@@ -12917,7 +12920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>235</v>
       </c>
@@ -12937,7 +12940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>238</v>
       </c>
@@ -12957,7 +12960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>240</v>
       </c>
@@ -12977,7 +12980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>242</v>
       </c>
@@ -12997,7 +13000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>248</v>
       </c>
@@ -13017,7 +13020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>250</v>
       </c>
@@ -13037,7 +13040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>252</v>
       </c>
@@ -13057,7 +13060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>258</v>
       </c>
@@ -13077,7 +13080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>274</v>
       </c>
@@ -13097,7 +13100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>275</v>
       </c>
@@ -13117,7 +13120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>294</v>
       </c>
@@ -13137,7 +13140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>221</v>
       </c>
@@ -13157,7 +13160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>223</v>
       </c>
@@ -13177,7 +13180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>225</v>
       </c>
@@ -13197,7 +13200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>226</v>
       </c>
@@ -13217,7 +13220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>227</v>
       </c>
@@ -13237,7 +13240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>228</v>
       </c>
@@ -13257,7 +13260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>230</v>
       </c>
@@ -13277,7 +13280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>232</v>
       </c>
@@ -13297,7 +13300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>234</v>
       </c>
@@ -13317,7 +13320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>236</v>
       </c>
@@ -13337,7 +13340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>241</v>
       </c>
@@ -13357,7 +13360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>249</v>
       </c>
@@ -13377,7 +13380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>254</v>
       </c>
@@ -13397,7 +13400,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>256</v>
       </c>
@@ -13417,7 +13420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>261</v>
       </c>
@@ -13437,7 +13440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>262</v>
       </c>
@@ -13457,7 +13460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>266</v>
       </c>
@@ -13477,7 +13480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>267</v>
       </c>
@@ -13497,7 +13500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>270</v>
       </c>
@@ -13517,7 +13520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>271</v>
       </c>
@@ -13537,7 +13540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>272</v>
       </c>
@@ -13557,7 +13560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>279</v>
       </c>
@@ -13577,7 +13580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>209</v>
       </c>
@@ -13597,7 +13600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>212</v>
       </c>
@@ -13617,7 +13620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>215</v>
       </c>
@@ -13637,7 +13640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>216</v>
       </c>
@@ -13657,7 +13660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>222</v>
       </c>
@@ -13677,7 +13680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>224</v>
       </c>
@@ -13697,7 +13700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>243</v>
       </c>
@@ -13717,7 +13720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>245</v>
       </c>
@@ -13737,7 +13740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>251</v>
       </c>
@@ -13757,7 +13760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>263</v>
       </c>
@@ -13777,7 +13780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>265</v>
       </c>
@@ -13797,7 +13800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>268</v>
       </c>
@@ -13817,7 +13820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>280</v>
       </c>
@@ -13837,7 +13840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>286</v>
       </c>
@@ -13857,7 +13860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>287</v>
       </c>
@@ -13877,7 +13880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>288</v>
       </c>
@@ -13897,7 +13900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>289</v>
       </c>
@@ -13917,7 +13920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>291</v>
       </c>
@@ -13937,7 +13940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>293</v>
       </c>
@@ -13957,7 +13960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>239</v>
       </c>
@@ -13977,7 +13980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>200</v>
       </c>
@@ -13997,7 +14000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>201</v>
       </c>
@@ -14017,7 +14020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>202</v>
       </c>
@@ -14037,7 +14040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>203</v>
       </c>
@@ -14057,7 +14060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>204</v>
       </c>
@@ -14077,7 +14080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>205</v>
       </c>
@@ -14097,7 +14100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>206</v>
       </c>
@@ -14117,7 +14120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>207</v>
       </c>
@@ -14137,7 +14140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>208</v>
       </c>
@@ -14157,7 +14160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>210</v>
       </c>
@@ -14177,7 +14180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>211</v>
       </c>
@@ -14197,7 +14200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>213</v>
       </c>
@@ -14217,7 +14220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>214</v>
       </c>
@@ -14237,7 +14240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>217</v>
       </c>
@@ -14257,7 +14260,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>218</v>
       </c>
@@ -14277,7 +14280,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>219</v>
       </c>
@@ -14297,7 +14300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>220</v>
       </c>
@@ -14317,7 +14320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>244</v>
       </c>
@@ -14337,7 +14340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>246</v>
       </c>
@@ -14357,7 +14360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>253</v>
       </c>
@@ -14377,7 +14380,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>257</v>
       </c>
@@ -14397,7 +14400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>260</v>
       </c>
@@ -14417,7 +14420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>264</v>
       </c>
@@ -14437,7 +14440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>269</v>
       </c>
@@ -14457,7 +14460,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>276</v>
       </c>
@@ -14477,7 +14480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>277</v>
       </c>
@@ -14497,7 +14500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>281</v>
       </c>
@@ -14517,7 +14520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>282</v>
       </c>
@@ -14537,7 +14540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>283</v>
       </c>
@@ -14557,7 +14560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>284</v>
       </c>
@@ -14577,7 +14580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>285</v>
       </c>
@@ -14597,7 +14600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>290</v>
       </c>
@@ -14617,7 +14620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>292</v>
       </c>
@@ -14637,7 +14640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>229</v>
       </c>
@@ -14657,7 +14660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>237</v>
       </c>
@@ -14677,7 +14680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>247</v>
       </c>
@@ -14697,7 +14700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>255</v>
       </c>
@@ -14717,7 +14720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>259</v>
       </c>
@@ -14737,7 +14740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>273</v>
       </c>
@@ -14757,7 +14760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>278</v>
       </c>
@@ -14780,7 +14783,7 @@
   </sheetData>
   <autoFilter ref="A1:I400" xr:uid="{F2932DD1-FA9E-416E-B4CD-BA827FBD2940}"/>
   <dataConsolidate/>
-  <conditionalFormatting sqref="H2:H4 H13 H29 H31:H33 H35 H37:H47 H57:H59 I152 E2:G400 I126 I120 I122 I132 H100:H101">
+  <conditionalFormatting sqref="H2:H4 H13 H29 H31:H33 H35 H37:H47 H57:H59 I152 E2:G400 I126 I120 I122 I132 H100:H101 I148 I141">
     <cfRule type="containsText" dxfId="35" priority="47" operator="containsText" text="Favor">
       <formula>NOT(ISERROR(SEARCH("Favor",E2)))</formula>
     </cfRule>

</xml_diff>